<commit_message>
Added Varistor Alternate P/N, J16-J18 P/N
</commit_message>
<xml_diff>
--- a/PCB/BOM/H7864 BOM 2021.xlsx
+++ b/PCB/BOM/H7864 BOM 2021.xlsx
@@ -1,27 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GoogleDrive\VAX Museum\H7864\PCB Rev B\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GoogleDrive\VAX Museum\Projects\H7864\Production File\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E4C232D-5629-4757-ACA2-B9FBF03A0BD6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A59A6A9-F04A-4C20-865A-DF88FE666D9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Part List Report" sheetId="3" r:id="rId1"/>
     <sheet name="Project Information" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="163">
   <si>
     <t>Project Full Path</t>
   </si>
@@ -502,6 +512,15 @@
   </si>
   <si>
     <t>A, B</t>
+  </si>
+  <si>
+    <t>TE 640445-3 see note</t>
+  </si>
+  <si>
+    <t>V10E300P, MOV-10D471K</t>
+  </si>
+  <si>
+    <t>Note: J16-J18 can be populated with TE 640445-3, center pin must be removed. Orientation should match the wiring of loom J16-J18 for Live/Neutral connectios</t>
   </si>
 </sst>
 </file>
@@ -996,7 +1015,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1010,68 +1029,68 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1081,22 +1100,22 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="9" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1109,13 +1128,13 @@
     <xf numFmtId="0" fontId="11" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -1146,7 +1165,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1164,21 +1183,31 @@
     <xf numFmtId="0" fontId="13" fillId="6" borderId="18" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1592,24 +1621,24 @@
   </sheetPr>
   <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="3.1328125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="3.109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.3984375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="20.1328125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="10.38671875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" style="4" customWidth="1"/>
     <col min="5" max="6" width="31" style="1" customWidth="1"/>
     <col min="7" max="7" width="33" style="1" customWidth="1"/>
-    <col min="8" max="8" width="17.86328125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.88671875" style="1" customWidth="1"/>
     <col min="9" max="9" width="10" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.1328125" style="1"/>
+    <col min="10" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="12.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="14"/>
       <c r="B1" s="14"/>
       <c r="C1" s="5"/>
@@ -1620,7 +1649,7 @@
       <c r="H1" s="19"/>
       <c r="I1" s="23"/>
     </row>
-    <row r="2" spans="1:9" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="15"/>
       <c r="B2" s="41"/>
       <c r="C2" s="41" t="s">
@@ -1676,7 +1705,7 @@
       <c r="G5" s="31"/>
       <c r="H5" s="32"/>
     </row>
-    <row r="6" spans="1:9" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A6" s="15"/>
       <c r="B6" s="35"/>
       <c r="C6" s="35"/>
@@ -1686,7 +1715,7 @@
       <c r="G6" s="29"/>
       <c r="H6" s="37"/>
     </row>
-    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="15"/>
       <c r="B7" s="38"/>
       <c r="C7" s="38" t="s">
@@ -1702,7 +1731,7 @@
       <c r="G7" s="31"/>
       <c r="H7" s="32"/>
     </row>
-    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="15"/>
       <c r="B8" s="34"/>
       <c r="C8" s="34" t="s">
@@ -1710,17 +1739,17 @@
       </c>
       <c r="D8" s="39">
         <f ca="1">TODAY()</f>
-        <v>44284</v>
+        <v>44889</v>
       </c>
       <c r="E8" s="40">
         <f ca="1">NOW()</f>
-        <v>44284.821481481478</v>
+        <v>44889.683402314811</v>
       </c>
       <c r="F8" s="40"/>
       <c r="G8" s="34"/>
       <c r="H8" s="32"/>
     </row>
-    <row r="9" spans="1:9" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="15"/>
       <c r="B9" s="49" t="s">
         <v>22</v>
@@ -1744,7 +1773,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="15"/>
       <c r="B10" s="47">
         <v>1</v>
@@ -1766,7 +1795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="15"/>
       <c r="B11" s="50">
         <v>2</v>
@@ -1788,7 +1817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="15"/>
       <c r="B12" s="47">
         <v>3</v>
@@ -1810,7 +1839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="15"/>
       <c r="B13" s="50">
         <v>4</v>
@@ -1834,7 +1863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="15"/>
       <c r="B14" s="47">
         <v>5</v>
@@ -1858,7 +1887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="15"/>
       <c r="B15" s="50">
         <v>6</v>
@@ -1882,7 +1911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="15"/>
       <c r="B16" s="47">
         <v>7</v>
@@ -1904,7 +1933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="15"/>
       <c r="B17" s="50">
         <v>8</v>
@@ -1928,7 +1957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="15"/>
       <c r="B18" s="47">
         <v>9</v>
@@ -1950,7 +1979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="15"/>
       <c r="B19" s="50">
         <v>10</v>
@@ -1972,7 +2001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="15"/>
       <c r="B20" s="47">
         <v>11</v>
@@ -1996,7 +2025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="15"/>
       <c r="B21" s="50">
         <v>12</v>
@@ -2020,7 +2049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="15"/>
       <c r="B22" s="47">
         <v>13</v>
@@ -2044,7 +2073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="15"/>
       <c r="B23" s="50">
         <v>14</v>
@@ -2064,7 +2093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="15"/>
       <c r="B24" s="47">
         <v>15</v>
@@ -2084,7 +2113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" s="15"/>
       <c r="B25" s="50">
         <v>16</v>
@@ -2104,7 +2133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="15"/>
       <c r="B26" s="47">
         <v>17</v>
@@ -2112,7 +2141,9 @@
       <c r="C26" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="D26" s="48"/>
+      <c r="D26" s="48" t="s">
+        <v>160</v>
+      </c>
       <c r="E26" s="48" t="s">
         <v>117</v>
       </c>
@@ -2124,7 +2155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A27" s="15"/>
       <c r="B27" s="50">
         <v>18</v>
@@ -2144,7 +2175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A28" s="15"/>
       <c r="B28" s="47">
         <v>19</v>
@@ -2152,7 +2183,9 @@
       <c r="C28" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="D28" s="48"/>
+      <c r="D28" s="48" t="s">
+        <v>160</v>
+      </c>
       <c r="E28" s="48" t="s">
         <v>117</v>
       </c>
@@ -2164,7 +2197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="15"/>
       <c r="B29" s="50">
         <v>20</v>
@@ -2186,7 +2219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="15"/>
       <c r="B30" s="47">
         <v>21</v>
@@ -2206,7 +2239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A31" s="15"/>
       <c r="B31" s="50">
         <v>22</v>
@@ -2226,7 +2259,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A32" s="15"/>
       <c r="B32" s="47">
         <v>23</v>
@@ -2246,7 +2279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A33" s="15"/>
       <c r="B33" s="50">
         <v>24</v>
@@ -2266,7 +2299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A34" s="15"/>
       <c r="B34" s="47">
         <v>25</v>
@@ -2284,13 +2317,13 @@
         <v>154</v>
       </c>
       <c r="G34" s="48" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="H34" s="52">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A35" s="15"/>
       <c r="B35" s="50">
         <v>26</v>
@@ -2312,7 +2345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A36" s="15"/>
       <c r="B36" s="47">
         <v>27</v>
@@ -2332,7 +2365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A37" s="15"/>
       <c r="B37" s="50">
         <v>28</v>
@@ -2354,7 +2387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A38" s="15"/>
       <c r="B38" s="47">
         <v>29</v>
@@ -2374,7 +2407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A39" s="15"/>
       <c r="B39" s="50">
         <v>30</v>
@@ -2396,7 +2429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A40" s="15"/>
       <c r="B40" s="47">
         <v>31</v>
@@ -2420,7 +2453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A41" s="15"/>
       <c r="B41" s="50">
         <v>32</v>
@@ -2442,7 +2475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A42" s="15"/>
       <c r="B42" s="47">
         <v>33</v>
@@ -2464,7 +2497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A43" s="15"/>
       <c r="B43" s="50">
         <v>34</v>
@@ -2486,7 +2519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A44" s="15"/>
       <c r="B44" s="47">
         <v>35</v>
@@ -2510,7 +2543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A45" s="15"/>
       <c r="B45" s="50">
         <v>36</v>
@@ -2532,7 +2565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A46" s="15"/>
       <c r="B46" s="47">
         <v>37</v>
@@ -2556,7 +2589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A47" s="15"/>
       <c r="B47" s="50">
         <v>38</v>
@@ -2580,7 +2613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A48" s="15"/>
       <c r="B48" s="47">
         <v>39</v>
@@ -2602,7 +2635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A49" s="15"/>
       <c r="B49" s="50">
         <v>40</v>
@@ -2626,7 +2659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A50" s="15"/>
       <c r="B50" s="47">
         <v>41</v>
@@ -2648,7 +2681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A51" s="15"/>
       <c r="B51" s="50">
         <v>42</v>
@@ -2672,7 +2705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A52" s="15"/>
       <c r="B52" s="47">
         <v>43</v>
@@ -2694,7 +2727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A53" s="15"/>
       <c r="B53" s="50">
         <v>44</v>
@@ -2716,7 +2749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A54" s="15"/>
       <c r="B54" s="47">
         <v>45</v>
@@ -2740,7 +2773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A55" s="15"/>
       <c r="B55" s="50">
         <v>46</v>
@@ -2764,7 +2797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A56" s="15"/>
       <c r="B56" s="47">
         <v>47</v>
@@ -2786,7 +2819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A57" s="15"/>
       <c r="B57" s="50">
         <v>48</v>
@@ -2808,7 +2841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A58" s="15"/>
       <c r="B58" s="47">
         <v>49</v>
@@ -2830,7 +2863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A59" s="15"/>
       <c r="B59" s="50">
         <v>50</v>
@@ -2852,7 +2885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A60" s="15"/>
       <c r="B60" s="47">
         <v>51</v>
@@ -2874,7 +2907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A61" s="15"/>
       <c r="B61" s="50">
         <v>52</v>
@@ -2896,7 +2929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A62" s="15"/>
       <c r="B62" s="47">
         <v>53</v>
@@ -2918,7 +2951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A63" s="15"/>
       <c r="B63" s="50">
         <v>54</v>
@@ -2942,7 +2975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A64" s="15"/>
       <c r="B64" s="47">
         <v>55</v>
@@ -2966,7 +2999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A65" s="15"/>
       <c r="B65" s="50">
         <v>56</v>
@@ -2988,7 +3021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="13.15" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A66" s="15"/>
       <c r="B66" s="64" t="s">
         <v>20</v>
@@ -3004,7 +3037,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A67" s="15"/>
       <c r="B67" s="11"/>
       <c r="C67" s="11"/>
@@ -3014,17 +3047,19 @@
       <c r="G67" s="10"/>
       <c r="H67" s="20"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A68" s="15"/>
-      <c r="B68" s="11"/>
-      <c r="C68" s="11"/>
-      <c r="D68" s="13"/>
-      <c r="E68" s="9"/>
-      <c r="F68" s="9"/>
-      <c r="G68" s="11"/>
-      <c r="H68" s="21"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B68" s="68" t="s">
+        <v>162</v>
+      </c>
+      <c r="C68" s="66"/>
+      <c r="D68" s="66"/>
+      <c r="E68" s="66"/>
+      <c r="F68" s="66"/>
+      <c r="G68" s="66"/>
+      <c r="H68" s="67"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A69" s="15"/>
       <c r="B69" s="11"/>
       <c r="C69" s="11"/>
@@ -3034,7 +3069,7 @@
       <c r="G69" s="11"/>
       <c r="H69" s="21"/>
     </row>
-    <row r="70" spans="1:8" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:8" ht="12.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A70" s="15"/>
       <c r="B70" s="45"/>
       <c r="C70" s="18"/>
@@ -3044,21 +3079,22 @@
       <c r="G70" s="18"/>
       <c r="H70" s="22"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B68:H68"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.46" right="0.36" top="0.57999999999999996" bottom="1" header="0.5" footer="0.5"/>
@@ -3078,13 +3114,13 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="110.59765625" customWidth="1"/>
+    <col min="2" max="2" width="110.609375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="13.15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
@@ -3092,7 +3128,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="13.15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
@@ -3100,7 +3136,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="13.15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" s="44" t="s">
         <v>2</v>
       </c>
@@ -3108,7 +3144,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="13.15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" s="43" t="s">
         <v>3</v>
       </c>
@@ -3116,7 +3152,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="13.15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" s="44" t="s">
         <v>4</v>
       </c>
@@ -3124,7 +3160,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="13.15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" s="43" t="s">
         <v>5</v>
       </c>
@@ -3132,7 +3168,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="13.15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A7" s="44" t="s">
         <v>6</v>
       </c>
@@ -3140,7 +3176,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="13.15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8" s="43" t="s">
         <v>7</v>
       </c>
@@ -3148,7 +3184,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="13.15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A9" s="44" t="s">
         <v>8</v>
       </c>
@@ -3156,7 +3192,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="13.15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A10" s="43" t="s">
         <v>9</v>
       </c>
@@ -3164,7 +3200,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="13.15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A11" s="44" t="s">
         <v>10</v>
       </c>
@@ -3172,7 +3208,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="13.15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A12" s="43" t="s">
         <v>11</v>
       </c>
@@ -3180,7 +3216,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="13.15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A13" s="44" t="s">
         <v>12</v>
       </c>
@@ -3188,7 +3224,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="13.15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A14" s="43" t="s">
         <v>13</v>
       </c>

</xml_diff>